<commit_message>
Mudança no código do relatorio de captacao
</commit_message>
<xml_diff>
--- a/historicocomissoes/202404/cambio/cambio.xlsx
+++ b/historicocomissoes/202404/cambio/cambio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f97ab02c6af1f0/Miha/Comissões/PJ2/03.2024 - XP P2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76f97ab02c6af1f0/Miha/Comissões/PJ2/04.2024 - XP P2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B012F1-9B56-48A0-971C-7424984BE187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0727810-9349-4A5E-A45B-B948292B593C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35985" yWindow="4890" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
   <si>
     <t>Classificação</t>
   </si>
@@ -73,85 +73,127 @@
     <t>USD</t>
   </si>
   <si>
-    <t>63750</t>
-  </si>
-  <si>
-    <t>TX.CLIENTE 4,99930 | TX.BASE 4,95230</t>
+    <t>21774,18</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,08655 | TX.BASE 5,07640</t>
+  </si>
+  <si>
+    <t>A70995</t>
+  </si>
+  <si>
+    <t>12/04/2024</t>
+  </si>
+  <si>
+    <t>25986,59</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,12471 | TX.BASE 5,10990</t>
+  </si>
+  <si>
+    <t>30/04/2024</t>
+  </si>
+  <si>
+    <t>Compra</t>
+  </si>
+  <si>
+    <t>1000045,47</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,17634 | TX.BASE 5,22860</t>
+  </si>
+  <si>
+    <t>18/04/2024</t>
+  </si>
+  <si>
+    <t>1000950</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,12131 | TX.BASE 5,20080</t>
+  </si>
+  <si>
+    <t>22/04/2024</t>
+  </si>
+  <si>
+    <t>2999950</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,02800 | TX.BASE 5,10910</t>
+  </si>
+  <si>
+    <t>29/04/2024</t>
+  </si>
+  <si>
+    <t>Mercado Internacional</t>
+  </si>
+  <si>
+    <t>4661,05</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,26371 | TX.BASE 5,25320</t>
+  </si>
+  <si>
+    <t>A22579</t>
+  </si>
+  <si>
+    <t>08/04/2024</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>51099,5</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,55391 | TX.BASE 5,47191</t>
+  </si>
+  <si>
+    <t>51999,49</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,22231 | TX.BASE 5,17110</t>
   </si>
   <si>
     <t>A67370</t>
   </si>
   <si>
-    <t>05/03/2024</t>
-  </si>
-  <si>
-    <t>Compra</t>
-  </si>
-  <si>
-    <t>1000000</t>
-  </si>
-  <si>
-    <t>TX.CLIENTE 4,94890 | TX.BASE 4,98630</t>
-  </si>
-  <si>
-    <t>A70995</t>
-  </si>
-  <si>
-    <t>25/03/2024</t>
-  </si>
-  <si>
-    <t>43518,13</t>
-  </si>
-  <si>
-    <t>TX.CLIENTE 5,05230 | TX.BASE 5,00030</t>
-  </si>
-  <si>
-    <t>28/03/2024</t>
-  </si>
-  <si>
-    <t>195260</t>
-  </si>
-  <si>
-    <t>TX.CLIENTE 4,94840 | TX.BASE 4,98780</t>
+    <t>Campanha Câmbio</t>
+  </si>
+  <si>
+    <t>Bonificação Exclusiva</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>1000</t>
   </si>
   <si>
-    <t>TX.CLIENTE 5,23814 | TX.BASE 4,98870</t>
+    <t>TX.CLIENTE 5,39742 | TX.BASE 5,17440</t>
   </si>
   <si>
     <t>A72673</t>
   </si>
   <si>
-    <t>18/03/2024</t>
-  </si>
-  <si>
-    <t>Campanha Câmbio</t>
-  </si>
-  <si>
-    <t>Bonificação Exclusiva</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>31/03/2024</t>
-  </si>
-  <si>
-    <t>FINANCEIRO-VD</t>
-  </si>
-  <si>
-    <t>577,51</t>
-  </si>
-  <si>
-    <t>TX.CLIENTE 5,13812 | TX.BASE 5,02505</t>
-  </si>
-  <si>
-    <t>A72495</t>
-  </si>
-  <si>
-    <t>22/03/2024</t>
+    <t>TX.CLIENTE 5,32342 | TX.BASE 5,11130</t>
+  </si>
+  <si>
+    <t>26/04/2024</t>
+  </si>
+  <si>
+    <t>338931,03</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 5,09886 | TX.BASE 5,11420</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>2000,08</t>
+  </si>
+  <si>
+    <t>TX.CLIENTE 6,42900 | TX.BASE 6,39633</t>
   </si>
 </sst>
 </file>
@@ -521,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -593,7 +635,7 @@
         <v>18</v>
       </c>
       <c r="G2">
-        <v>5248748</v>
+        <v>7245059</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
@@ -602,16 +644,16 @@
         <v>20</v>
       </c>
       <c r="J2" s="1">
-        <v>2996.12</v>
+        <v>221.07</v>
       </c>
       <c r="K2" s="1">
-        <v>2856.8</v>
+        <v>210.79</v>
       </c>
       <c r="L2" s="1">
         <v>50</v>
       </c>
       <c r="M2" s="1">
-        <v>1428.4</v>
+        <v>105.39</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -622,37 +664,37 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3">
+        <v>7245059</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="G3">
-        <v>15021649</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
       <c r="J3" s="1">
-        <v>37397</v>
+        <v>384.83</v>
       </c>
       <c r="K3" s="1">
-        <v>35658.03</v>
+        <v>366.94</v>
       </c>
       <c r="L3" s="1">
         <v>50</v>
       </c>
       <c r="M3" s="1">
-        <v>17829.009999999998</v>
+        <v>183.47</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -663,37 +705,37 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
       <c r="G4">
-        <v>2318067</v>
+        <v>15021649</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="1">
-        <v>2263.08</v>
+        <v>52260.37</v>
       </c>
       <c r="K4" s="1">
-        <v>2157.84</v>
+        <v>49830.26</v>
       </c>
       <c r="L4" s="1">
         <v>50</v>
       </c>
       <c r="M4" s="1">
-        <v>1078.92</v>
+        <v>24915.13</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -704,37 +746,37 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
       </c>
       <c r="G5">
         <v>15021649</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1">
-        <v>7694.02</v>
+        <v>79565.509999999995</v>
       </c>
       <c r="K5" s="1">
-        <v>7336.24</v>
+        <v>75865.710000000006</v>
       </c>
       <c r="L5" s="1">
         <v>50</v>
       </c>
       <c r="M5" s="1">
-        <v>3668.12</v>
+        <v>37932.85</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -745,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -757,25 +799,25 @@
         <v>32</v>
       </c>
       <c r="G6">
-        <v>5092910</v>
+        <v>15021649</v>
       </c>
       <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
       <c r="J6" s="1">
-        <v>249.44</v>
+        <v>243295.94</v>
       </c>
       <c r="K6" s="1">
-        <v>237.84</v>
+        <v>231982.68</v>
       </c>
       <c r="L6" s="1">
         <v>50</v>
       </c>
       <c r="M6" s="1">
-        <v>118.92</v>
+        <v>115991.34</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -783,37 +825,40 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7">
+        <v>506548</v>
+      </c>
+      <c r="H7" t="s">
         <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
       </c>
       <c r="I7" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="1">
-        <v>9837.86</v>
+        <v>438.89</v>
       </c>
       <c r="K7" s="1">
-        <v>9837.86</v>
+        <v>418.48</v>
       </c>
       <c r="L7" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M7" s="1">
-        <v>9837.86</v>
+        <v>209.24</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
@@ -824,10 +869,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -836,25 +881,306 @@
         <v>41</v>
       </c>
       <c r="G8">
-        <v>6594577</v>
+        <v>7298496</v>
       </c>
       <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="1">
+        <v>4190.3599999999997</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3995.51</v>
+      </c>
+      <c r="L8" s="1">
+        <v>50</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1997.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="I8" t="s">
+      <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="1">
-        <v>65.3</v>
-      </c>
-      <c r="K8" s="1">
-        <v>62.26</v>
-      </c>
-      <c r="L8" s="1">
-        <v>50</v>
-      </c>
-      <c r="M8" s="1">
-        <v>31.13</v>
+      <c r="G9">
+        <v>2318067</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2662.68</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2538.87</v>
+      </c>
+      <c r="L9" s="1">
+        <v>50</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1269.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-4777.8900000000003</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-4777.8900000000003</v>
+      </c>
+      <c r="L10" s="1">
+        <v>100</v>
+      </c>
+      <c r="M10" s="1">
+        <v>-4777.8900000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>5092910</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1">
+        <v>223.01</v>
+      </c>
+      <c r="K11" s="1">
+        <v>212.64</v>
+      </c>
+      <c r="L11" s="1">
+        <v>50</v>
+      </c>
+      <c r="M11" s="1">
+        <v>106.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12">
+        <v>5092910</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="1">
+        <v>212.11</v>
+      </c>
+      <c r="K12" s="1">
+        <v>202.25</v>
+      </c>
+      <c r="L12" s="1">
+        <v>50</v>
+      </c>
+      <c r="M12" s="1">
+        <v>101.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1">
+        <v>38402.58</v>
+      </c>
+      <c r="K13" s="1">
+        <v>38402.58</v>
+      </c>
+      <c r="L13" s="1">
+        <v>100</v>
+      </c>
+      <c r="M13" s="1">
+        <v>38402.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14">
+        <v>9594189</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5200.21</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4958.3999999999996</v>
+      </c>
+      <c r="L14" s="1">
+        <v>50</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2479.1999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15">
+        <v>3985621</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1">
+        <v>65.33</v>
+      </c>
+      <c r="K15" s="1">
+        <v>62.29</v>
+      </c>
+      <c r="L15" s="1">
+        <v>50</v>
+      </c>
+      <c r="M15" s="1">
+        <v>31.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>